<commit_message>
New laptop + JSHS updates.
</commit_message>
<xml_diff>
--- a/results/JSHS/Summary.xlsx
+++ b/results/JSHS/Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="-180" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
   <si>
     <t>start</t>
   </si>
@@ -40,6 +40,57 @@
   </si>
   <si>
     <t>fp</t>
+  </si>
+  <si>
+    <t>proteins</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>TNFRSF1B</t>
+  </si>
+  <si>
+    <t>STAT1</t>
+  </si>
+  <si>
+    <t>TNF</t>
+  </si>
+  <si>
+    <t>TRADD</t>
+  </si>
+  <si>
+    <t>TRAF2</t>
+  </si>
+  <si>
+    <t>FADD</t>
+  </si>
+  <si>
+    <t>SYK</t>
+  </si>
+  <si>
+    <t>PTK2</t>
+  </si>
+  <si>
+    <t>MAP3K5</t>
+  </si>
+  <si>
+    <t>TNFRSF1A</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>green = positive</t>
+  </si>
+  <si>
+    <t>red = fp</t>
+  </si>
+  <si>
+    <t>white = negative</t>
+  </si>
+  <si>
+    <t>X = equals, lower triangle</t>
   </si>
 </sst>
 </file>
@@ -378,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +440,7 @@
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -405,8 +456,17 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -422,8 +482,17 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -440,8 +509,17 @@
       <c r="E3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A46" si="0">A3+1</f>
         <v>3</v>
@@ -461,8 +539,17 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -479,8 +566,17 @@
       <c r="E5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -497,8 +593,17 @@
       <c r="E6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -515,8 +620,17 @@
       <c r="E7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -533,8 +647,17 @@
       <c r="E8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -554,8 +677,17 @@
       <c r="F9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -572,8 +704,17 @@
       <c r="E10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -590,8 +731,17 @@
       <c r="E11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -609,7 +759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -629,8 +779,11 @@
       <c r="F13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -647,8 +800,11 @@
       <c r="E14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -665,8 +821,11 @@
       <c r="E15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -682,6 +841,9 @@
       </c>
       <c r="E16" t="s">
         <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>